<commit_message>
spring security configuration, users, validation
</commit_message>
<xml_diff>
--- a/ecom/src/main/resources/static/products.xlsx
+++ b/ecom/src/main/resources/static/products.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karol\Desktop\ecom\src\main\resources\static\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karol\Desktop\back+front\ecom\src\main\resources\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF330481-7462-413E-95F1-EA5AD8B4B5B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3B19688-A062-425A-94BF-CC2BEA1ABE7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-1308" windowWidth="23256" windowHeight="12456" xr2:uid="{D7ECC196-771A-4C8D-AF28-361FF4117F14}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D7ECC196-771A-4C8D-AF28-361FF4117F14}"/>
   </bookViews>
   <sheets>
     <sheet name="asortyment" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t>id</t>
   </si>
@@ -59,18 +59,9 @@
     <t>type</t>
   </si>
   <si>
-    <t>img</t>
-  </si>
-  <si>
     <t>video</t>
   </si>
   <si>
-    <t>https://video.aliexpress-media.com/play/u/ae_sg_item/3298043957/p/1/e/6/t/10301/1100174480699.mp4?from=chrome&amp;amp;definition=h265</t>
-  </si>
-  <si>
-    <t>https://ae01.alicdn.com/kf/S33cff507da554c48bfe6bd03c80e73dfW/Spinpoler-Firebomb-Soft-Swimbait-17-5cm-22cm-przyn-ta-d-ugie-faliste-ogon-du-y-szczupak.jpg</t>
-  </si>
-  <si>
     <t>colors</t>
   </si>
   <si>
@@ -83,9 +74,6 @@
     <t>S11ed721bd72a49b1b35d8a76bd08d30fO/Spinpoler-Firebomb-Soft-Swimbait-17-5cm-22cm-przyn-ta-d-ugie-faliste-ogon-du-y-szczupak.jpg_640x640.jpg+Sbbcff94f0135408bbf0be1c5f51fe695B/Spinpoler-Firebomb-Soft-Swimbait-17-5cm-22cm-przyn-ta-d-ugie-faliste-ogon-du-y-szczupak.jpg_640x640.jpg+S4e7fbb710aad4fdf8a15d08956749394o/Spinpoler-Firebomb-Soft-Swimbait-17-5cm-22cm-przyn-ta-d-ugie-faliste-ogon-du-y-szczupak.jpg_640x640.jpg+S108c014cb50848dba0080694983fb282G/Spinpoler-Firebomb-Soft-Swimbait-17-5cm-22cm-przyn-ta-d-ugie-faliste-ogon-du-y-szczupak.jpg_640x640.jpg+S450ccbca2e79459ebc143c3a37e34820h/Spinpoler-Firebomb-Soft-Swimbait-17-5cm-22cm-przyn-ta-d-ugie-faliste-ogon-du-y-szczupak.jpg_640x640.jpg+S218c26f355c44df69d6381cbb307e596T/Spinpoler-Firebomb-Soft-Swimbait-17-5cm-22cm-przyn-ta-d-ugie-faliste-ogon-du-y-szczupak.jpg_640x640.jpg+Sb111f401ed5f48ca8045c8a9c248b9a4H/Spinpoler-Firebomb-Soft-Swimbait-17-5cm-22cm-przyn-ta-d-ugie-faliste-ogon-du-y-szczupak.jpg_640x640.jpg+S6819263774af4344a0d8105d0667fa33z/Spinpoler-Firebomb-Soft-Swimbait-17-5cm-22cm-przyn-ta-d-ugie-faliste-ogon-du-y-szczupak.jpg_640x640.jpg</t>
   </si>
   <si>
-    <t>https://video.aliexpress-media.com/play/u/ae_sg_item/3298043957/p/1/e/6/t/10301/1100174480699.mp4?from=chrome&amp;amp;definition=h266</t>
-  </si>
-  <si>
     <t>weight</t>
   </si>
   <si>
@@ -107,38 +95,29 @@
     <t>Akcesoria</t>
   </si>
   <si>
-    <t>https://video.aliexpress-media.com/play/u/ae_sg_item/3298043957/p/1/e/6/t/10301/1100116273060.mp4?from=chrome&amp;amp;definition=h265</t>
-  </si>
-  <si>
-    <t>https://ae01.alicdn.com/kf/S244087bb1e1549948d637fcc6fbbc5bfJ.jpg</t>
-  </si>
-  <si>
     <t>Wielofunkcyjne szczypce do usuwania haczyków. Uchwyt Lip Trigger Clamp. Wytrzymały materiał ABS</t>
   </si>
   <si>
     <t>Rak</t>
   </si>
   <si>
-    <t>https://ae01.alicdn.com/kf/S80097b70cef741cdb9f94762869bbef5L.jpg</t>
-  </si>
-  <si>
     <t>S2b02940884524c3f9c8b6542a6b68667W.jpg+S5361887a749a4d52ac20e995c662de878.jpg+S2f815daedf8543ada5c2ddb57fb9d9b3c.jpg+S0d91b634bdc9407183e03820c911b815D.jpg+Sc5533d38f1384905a0b793ccbbfeb2c55.jpg</t>
   </si>
   <si>
-    <t>https://video.aliexpress-media.com/play/u/ae_sg_item/3298043957/p/1/e/6/t/10301/1100217540643.mp4?from=chrome&amp;amp;definition=h265</t>
-  </si>
-  <si>
     <t>Sb313019a4e6d4bbdbaf64193bc2fce04d.jpg+Sd397f11eacd443d686c619f25cb05325q.jpg+S825de5c95fb74461a31a64ab87ec2dc7i.jpg+S510ff15d33304d888b10c3fbf67e5540t.jpg+Sae1ea579296c4cddb85ff4da13fe5f56B.jpg+S3be1779bd88d4ac1aefe5fe869c3b7cdA.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Świetna mała gumowa przynęta na rzeki i jeziora </t>
+  </si>
+  <si>
+    <t>cena zakupu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -158,6 +137,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="238"/>
@@ -185,10 +171,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperłącze" xfId="1" builtinId="8"/>
@@ -526,20 +513,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2A0C5A3-47CF-415F-B5BD-342042C3B21A}">
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="149.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="130.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="130.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" customWidth="1"/>
     <col min="12" max="12" width="112" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -550,19 +537,19 @@
         <v>6</v>
       </c>
       <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
-        <v>11</v>
-      </c>
       <c r="G1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="I1" t="s">
         <v>2</v>
@@ -571,16 +558,16 @@
         <v>3</v>
       </c>
       <c r="K1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" t="s">
         <v>16</v>
       </c>
-      <c r="L1" t="s">
-        <v>17</v>
-      </c>
-      <c r="M1" t="s">
-        <v>20</v>
-      </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -590,17 +577,15 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="D2" s="3">
+        <v>40.380000000000003</v>
+      </c>
+      <c r="E2" s="1"/>
       <c r="F2" s="2">
         <v>8</v>
       </c>
       <c r="G2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H2" s="2">
         <v>17.5</v>
@@ -608,20 +593,21 @@
       <c r="I2" s="2">
         <v>2</v>
       </c>
-      <c r="J2">
-        <v>59.99</v>
+      <c r="J2" s="2">
+        <f>INT(D2*1.25) + 0.99</f>
+        <v>50.99</v>
       </c>
       <c r="K2" s="2">
         <v>30</v>
       </c>
       <c r="L2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="M2">
         <v>59.99</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -631,17 +617,15 @@
       <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="D3" s="3">
+        <v>61.14</v>
+      </c>
+      <c r="E3" s="1"/>
       <c r="F3" s="2">
         <v>8</v>
       </c>
       <c r="G3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H3" s="2">
         <v>22</v>
@@ -649,40 +633,39 @@
       <c r="I3" s="2">
         <v>2</v>
       </c>
-      <c r="J3">
-        <v>79.989999999999995</v>
+      <c r="J3" s="2">
+        <f t="shared" ref="J3:J6" si="0">INT(D3*1.25) + 0.99</f>
+        <v>76.989999999999995</v>
       </c>
       <c r="K3" s="2">
         <v>55</v>
       </c>
       <c r="L3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="M3">
         <v>79.989999999999995</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>23</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1"/>
       <c r="F4" s="2">
         <v>5</v>
       </c>
       <c r="G4" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="H4" s="2">
         <v>20</v>
@@ -690,40 +673,39 @@
       <c r="I4" s="2">
         <v>1</v>
       </c>
-      <c r="J4">
-        <v>49.99</v>
+      <c r="J4" s="2">
+        <f t="shared" si="0"/>
+        <v>0.99</v>
       </c>
       <c r="K4" s="2">
         <v>59</v>
       </c>
       <c r="L4" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="M4">
         <v>49.99</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="D5" s="3">
+        <v>15.34</v>
+      </c>
+      <c r="E5" s="1"/>
       <c r="F5" s="2">
         <v>6</v>
       </c>
       <c r="G5" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="H5" s="2">
         <v>6.5</v>
@@ -732,39 +714,38 @@
         <v>5</v>
       </c>
       <c r="J5" s="2">
-        <v>40.99</v>
+        <f t="shared" si="0"/>
+        <v>19.989999999999998</v>
       </c>
       <c r="K5" s="2">
         <v>4</v>
       </c>
       <c r="L5" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="M5" s="2">
         <v>40.99</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="D6" s="3">
+        <v>15.34</v>
+      </c>
+      <c r="E6" s="1"/>
       <c r="F6" s="2">
         <v>6</v>
       </c>
       <c r="G6" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="H6" s="2">
         <v>6.5</v>
@@ -773,13 +754,14 @@
         <v>5</v>
       </c>
       <c r="J6" s="2">
-        <v>40.99</v>
+        <f t="shared" si="0"/>
+        <v>19.989999999999998</v>
       </c>
       <c r="K6" s="2">
         <v>4</v>
       </c>
       <c r="L6" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="M6" s="2">
         <v>40.99</v>
@@ -787,18 +769,6 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{7F78501C-97A3-4748-B5F8-7B882BB6A4ED}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{972A9B61-22DA-4C00-AB30-9E92E015E373}"/>
-    <hyperlink ref="D3" r:id="rId3" xr:uid="{92819A4B-C3CD-4369-BF6C-3720AF2D5F2D}"/>
-    <hyperlink ref="E3" r:id="rId4" display="https://video.aliexpress-media.com/play/u/ae_sg_item/3298043957/p/1/e/6/t/10301/1100174480699.mp4?from=chrome&amp;amp;definition=h265" xr:uid="{B98C3D74-E928-45F9-A197-11A4EB6ACA84}"/>
-    <hyperlink ref="E4" r:id="rId5" xr:uid="{B380FCC4-93F0-4E94-A3AA-0E68C87DDE44}"/>
-    <hyperlink ref="D4" r:id="rId6" xr:uid="{9CF36F87-03D7-4EF2-B7F2-5FA31BE8A739}"/>
-    <hyperlink ref="D5" r:id="rId7" xr:uid="{7D24B628-8F19-4705-9440-9338927F5F3A}"/>
-    <hyperlink ref="E5" r:id="rId8" xr:uid="{F7ADA14B-28B0-493F-A46D-F2223DA80CB8}"/>
-    <hyperlink ref="D6" r:id="rId9" xr:uid="{3660D3FB-C8EF-4D8F-8E70-9E68608C0C85}"/>
-    <hyperlink ref="E6" r:id="rId10" xr:uid="{9A92A0C3-A94C-4592-9331-89789FB977DF}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>